<commit_message>
saved changes to results reformat
</commit_message>
<xml_diff>
--- a/reformat_results.xlsx
+++ b/reformat_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="880" windowWidth="23080" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="1900" yWindow="760" windowWidth="23080" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -775,11 +775,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1801718208"/>
-        <c:axId val="-1868115712"/>
+        <c:axId val="-1200114208"/>
+        <c:axId val="-1192608656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1801718208"/>
+        <c:axId val="-1200114208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1868115712"/>
+        <c:crossAx val="-1192608656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -830,7 +830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1868115712"/>
+        <c:axId val="-1192608656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +880,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1801718208"/>
+        <c:crossAx val="-1200114208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1557,11 +1557,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1843094560"/>
-        <c:axId val="-1851418400"/>
+        <c:axId val="-1200586384"/>
+        <c:axId val="-1851782896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1843094560"/>
+        <c:axId val="-1200586384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1851418400"/>
+        <c:crossAx val="-1851782896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1612,7 +1612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1851418400"/>
+        <c:axId val="-1851782896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1662,7 +1662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1843094560"/>
+        <c:crossAx val="-1200586384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2339,11 +2339,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1794961632"/>
-        <c:axId val="-1799403040"/>
+        <c:axId val="-1791309888"/>
+        <c:axId val="-1791384160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1794961632"/>
+        <c:axId val="-1791309888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2386,7 +2386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1799403040"/>
+        <c:crossAx val="-1791384160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2394,7 +2394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1799403040"/>
+        <c:axId val="-1791384160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2445,7 +2445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1794961632"/>
+        <c:crossAx val="-1791309888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2954,11 +2954,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1584619648"/>
-        <c:axId val="-1793337920"/>
+        <c:axId val="-1194767152"/>
+        <c:axId val="-1865346448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1584619648"/>
+        <c:axId val="-1194767152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,7 +3001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1793337920"/>
+        <c:crossAx val="-1865346448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3009,7 +3009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1793337920"/>
+        <c:axId val="-1865346448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3059,7 +3059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1584619648"/>
+        <c:crossAx val="-1194767152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5702,8 +5702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>